<commit_message>
Fix TRE R66 f95a7adc7ef02c8dd9a8911eaaa0e64595201fa2
</commit_message>
<xml_diff>
--- a/feature/fix-TRER66/ig/ValueSet-sas-valueset-categorieetablissement.xlsx
+++ b/feature/fix-TRER66/ig/ValueSet-sas-valueset-categorieetablissement.xlsx
@@ -7,7 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
-    <sheet name="Include from TRE_R66-Categori" r:id="rId4" sheetId="2"/>
+    <sheet name="Include from " r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-08T16:11:11+00:00</t>
+    <t>2024-11-08T16:33:42+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -111,7 +111,7 @@
     <t>System URI</t>
   </si>
   <si>
-    <t>https://mos.esante.gouv.fr/NOS/TRE_R66-CategorieEtablissement/TRE_R66-CategorieEtablissement</t>
+    <t>https://mos.esante.gouv.fr/NOS/TRE_R66-CategorieEtablissement/FHIR/TRE-R66-CategorieEtablissement/</t>
   </si>
 </sst>
 </file>

</xml_diff>